<commit_message>
disallow different synopsis, panels, cohorts
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.26.mip.xlsx
+++ b/tests/fixtures/orderforms/1508.26.mip.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB349B-0928-7144-B5BD-A60A2BA437DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C742A9B-7BA9-C14A-8F32-2AA1123E0851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4340" yWindow="-19540" windowWidth="27840" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1180" yWindow="-20220" windowWidth="27840" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -5328,8 +5328,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -14108,8 +14108,8 @@
       <c r="P16" s="81"/>
       <c r="Q16" s="97"/>
       <c r="R16" s="48"/>
-      <c r="S16" s="163" t="s">
-        <v>82</v>
+      <c r="S16" s="166" t="s">
+        <v>505</v>
       </c>
       <c r="T16" s="120" t="s">
         <v>79</v>
@@ -15174,8 +15174,8 @@
       <c r="P17" s="81"/>
       <c r="Q17" s="97"/>
       <c r="R17" s="48"/>
-      <c r="S17" s="163" t="s">
-        <v>94</v>
+      <c r="S17" s="166" t="s">
+        <v>505</v>
       </c>
       <c r="T17" s="120" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Refactoring(structure): Move case fields from sample to case (#1497)
### Fixed:
* Move case fields from sample to case
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.26.mip.xlsx
+++ b/tests/fixtures/orderforms/1508.26.mip.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB349B-0928-7144-B5BD-A60A2BA437DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C742A9B-7BA9-C14A-8F32-2AA1123E0851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4340" yWindow="-19540" windowWidth="27840" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1180" yWindow="-20220" windowWidth="27840" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -5328,8 +5328,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -14108,8 +14108,8 @@
       <c r="P16" s="81"/>
       <c r="Q16" s="97"/>
       <c r="R16" s="48"/>
-      <c r="S16" s="163" t="s">
-        <v>82</v>
+      <c r="S16" s="166" t="s">
+        <v>505</v>
       </c>
       <c r="T16" s="120" t="s">
         <v>79</v>
@@ -15174,8 +15174,8 @@
       <c r="P17" s="81"/>
       <c r="Q17" s="97"/>
       <c r="R17" s="48"/>
-      <c r="S17" s="163" t="s">
-        <v>94</v>
+      <c r="S17" s="166" t="s">
+        <v>505</v>
       </c>
       <c r="T17" s="120" t="s">
         <v>79</v>

</xml_diff>